<commit_message>
fixed a problem with using True as header in Excel table
</commit_message>
<xml_diff>
--- a/example_data/Periodic Sine/example_2_modified.xlsx
+++ b/example_data/Periodic Sine/example_2_modified.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>x</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>measurement</t>
+  </si>
+  <si>
+    <t>truez</t>
   </si>
 </sst>
 </file>
@@ -404,7 +407,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,8 +419,8 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="b">
-        <v>1</v>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>

</xml_diff>